<commit_message>
Gestão de Informações de Exportação: É possível adicionar Proposta já existente com nº de Booking diferente e Proposta diferente e nº de Booking já existente também.
</commit_message>
<xml_diff>
--- a/CMSv4/Templates/gestao-informacoes-exportacao-template.xlsx
+++ b/CMSv4/Templates/gestao-informacoes-exportacao-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Larissa\source\repos\CMSv4.Alianca\CMSv4\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDED80A-F934-4119-AC8C-6BE3AB855E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECBC63D-219A-4216-A556-01F2793E8E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-2415" windowWidth="19440" windowHeight="15000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -396,14 +396,12 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="3"/>
-    <col min="2" max="2" width="8.5703125" style="6"/>
-    <col min="3" max="3" width="8.5703125" style="3"/>
+    <col min="1" max="3" width="8.5703125" style="3"/>
     <col min="4" max="4" width="8.5703125" style="6"/>
     <col min="5" max="7" width="8.5703125" style="3"/>
   </cols>
@@ -412,7 +410,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1"/>
@@ -421,343 +419,343 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
+      <c r="B2" s="4"/>
       <c r="D2" s="5"/>
       <c r="E2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
       <c r="D3" s="5"/>
       <c r="E3" s="4"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
+      <c r="B4" s="4"/>
       <c r="D4" s="5"/>
       <c r="E4" s="4"/>
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="D5" s="5"/>
       <c r="E5" s="4"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
+      <c r="B6" s="4"/>
       <c r="D6" s="5"/>
       <c r="E6" s="4"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
+      <c r="B7" s="4"/>
       <c r="D7" s="5"/>
       <c r="E7" s="4"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
+      <c r="B8" s="4"/>
       <c r="D8" s="5"/>
       <c r="E8" s="4"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
+      <c r="B9" s="4"/>
       <c r="D9" s="5"/>
       <c r="E9" s="4"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
+      <c r="B10" s="4"/>
       <c r="D10" s="5"/>
       <c r="E10" s="4"/>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
+      <c r="B11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="4"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
+      <c r="B12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="4"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
+      <c r="B13" s="4"/>
       <c r="D13" s="5"/>
       <c r="E13" s="4"/>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
+      <c r="B14" s="4"/>
       <c r="D14" s="5"/>
       <c r="E14" s="4"/>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
+      <c r="B15" s="4"/>
       <c r="D15" s="5"/>
       <c r="E15" s="4"/>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
+      <c r="B16" s="4"/>
       <c r="D16" s="5"/>
       <c r="E16" s="4"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
+      <c r="B17" s="4"/>
       <c r="D17" s="5"/>
       <c r="E17" s="4"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
+      <c r="B18" s="4"/>
       <c r="D18" s="5"/>
       <c r="E18" s="4"/>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
+      <c r="B19" s="4"/>
       <c r="D19" s="5"/>
       <c r="E19" s="4"/>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
+      <c r="B20" s="4"/>
       <c r="D20" s="5"/>
       <c r="E20" s="4"/>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
+      <c r="B21" s="4"/>
       <c r="D21" s="5"/>
       <c r="E21" s="4"/>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
+      <c r="B22" s="4"/>
       <c r="D22" s="5"/>
       <c r="E22" s="4"/>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
+      <c r="B23" s="4"/>
       <c r="D23" s="5"/>
       <c r="E23" s="4"/>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
+      <c r="B24" s="4"/>
       <c r="D24" s="5"/>
       <c r="E24" s="4"/>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
+      <c r="B25" s="4"/>
       <c r="D25" s="5"/>
       <c r="E25" s="4"/>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
+      <c r="B26" s="4"/>
       <c r="D26" s="5"/>
       <c r="E26" s="4"/>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
+      <c r="B27" s="4"/>
       <c r="D27" s="5"/>
       <c r="E27" s="4"/>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="5"/>
+      <c r="B28" s="4"/>
       <c r="D28" s="5"/>
       <c r="E28" s="4"/>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
+      <c r="B29" s="4"/>
       <c r="D29" s="5"/>
       <c r="E29" s="4"/>
       <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
+      <c r="B30" s="4"/>
       <c r="D30" s="5"/>
       <c r="E30" s="4"/>
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
+      <c r="B31" s="4"/>
       <c r="D31" s="5"/>
       <c r="E31" s="4"/>
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
+      <c r="B32" s="4"/>
       <c r="D32" s="5"/>
       <c r="E32" s="4"/>
       <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
+      <c r="B33" s="4"/>
       <c r="D33" s="5"/>
       <c r="E33" s="4"/>
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="B34" s="5"/>
+      <c r="B34" s="4"/>
       <c r="D34" s="5"/>
       <c r="E34" s="4"/>
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
+      <c r="B35" s="4"/>
       <c r="D35" s="5"/>
       <c r="E35" s="4"/>
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="4"/>
       <c r="D36" s="5"/>
       <c r="E36" s="4"/>
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="4"/>
       <c r="D37" s="5"/>
       <c r="E37" s="4"/>
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="5"/>
+      <c r="B38" s="4"/>
       <c r="D38" s="5"/>
       <c r="E38" s="4"/>
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="B39" s="5"/>
+      <c r="B39" s="4"/>
       <c r="D39" s="5"/>
       <c r="E39" s="4"/>
       <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
-      <c r="B40" s="5"/>
+      <c r="B40" s="4"/>
       <c r="D40" s="5"/>
       <c r="E40" s="4"/>
       <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
-      <c r="B41" s="5"/>
+      <c r="B41" s="4"/>
       <c r="D41" s="5"/>
       <c r="E41" s="4"/>
       <c r="G41" s="4"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
-      <c r="B42" s="5"/>
+      <c r="B42" s="4"/>
       <c r="D42" s="5"/>
       <c r="E42" s="4"/>
       <c r="G42" s="4"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
-      <c r="B43" s="5"/>
+      <c r="B43" s="4"/>
       <c r="D43" s="5"/>
       <c r="E43" s="4"/>
       <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
-      <c r="B44" s="5"/>
+      <c r="B44" s="4"/>
       <c r="D44" s="5"/>
       <c r="E44" s="4"/>
       <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
-      <c r="B45" s="5"/>
+      <c r="B45" s="4"/>
       <c r="D45" s="5"/>
       <c r="E45" s="4"/>
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
-      <c r="B46" s="5"/>
+      <c r="B46" s="4"/>
       <c r="D46" s="5"/>
       <c r="E46" s="4"/>
       <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
-      <c r="B47" s="5"/>
+      <c r="B47" s="4"/>
       <c r="D47" s="5"/>
       <c r="E47" s="4"/>
       <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
-      <c r="B48" s="5"/>
+      <c r="B48" s="4"/>
       <c r="D48" s="5"/>
       <c r="E48" s="4"/>
       <c r="G48" s="4"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
-      <c r="B49" s="5"/>
+      <c r="B49" s="4"/>
       <c r="D49" s="5"/>
       <c r="E49" s="4"/>
       <c r="G49" s="4"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
-      <c r="B50" s="5"/>
+      <c r="B50" s="4"/>
       <c r="D50" s="5"/>
       <c r="E50" s="4"/>
       <c r="G50" s="4"/>

</xml_diff>